<commit_message>
added test case for handling javascript alerts
</commit_message>
<xml_diff>
--- a/testData/excel/InputTestData.xlsx
+++ b/testData/excel/InputTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>TCID</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>test_TCID_104_adding_products_to_shopping_cart_and_checkout</t>
+  </si>
+  <si>
+    <t>test_handle_javascript</t>
+  </si>
+  <si>
+    <t>set_text</t>
+  </si>
+  <si>
+    <t>sanket_tester</t>
   </si>
 </sst>
 </file>
@@ -201,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -224,17 +233,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +860,28 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>